<commit_message>
generating new whole experiment data
</commit_message>
<xml_diff>
--- a/code/params/100_graph_params.xlsx
+++ b/code/params/100_graph_params.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ku51015\CHMURA\mystuff\geaometricgraphproperties\code\params\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4D265-583C-4EA8-A2E0-FCA0992619CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27960" windowHeight="12600"/>
+    <workbookView xWindow="10540" yWindow="13570" windowWidth="13070" windowHeight="10910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>graph_id</t>
   </si>
@@ -32,51 +38,21 @@
   <si>
     <t>outside_prob</t>
   </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.07</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.12</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
       <charset val="238"/>
@@ -106,17 +82,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -154,7 +138,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -188,6 +172,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -222,9 +207,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -397,16 +383,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -436,11 +422,11 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
+      <c r="D2">
+        <v>0.4</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -453,11 +439,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
+      <c r="E3">
+        <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -470,11 +456,11 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -487,11 +473,11 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
+      <c r="D5">
+        <v>0.4</v>
+      </c>
+      <c r="E5">
+        <v>0.08</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -504,11 +490,11 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
+      <c r="D6">
+        <v>0.4</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -521,11 +507,11 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+      <c r="E7">
+        <v>0.12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -538,11 +524,11 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
+      <c r="D8">
+        <v>0.35</v>
+      </c>
+      <c r="E8">
+        <v>0.06</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -555,11 +541,11 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
+      <c r="D9">
+        <v>0.3</v>
+      </c>
+      <c r="E9">
+        <v>0.02</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -572,11 +558,11 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
+      <c r="D10">
+        <v>0.4</v>
+      </c>
+      <c r="E10">
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -589,11 +575,11 @@
       <c r="C11">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
+      <c r="D11">
+        <v>0.4</v>
+      </c>
+      <c r="E11">
+        <v>0.02</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -606,11 +592,11 @@
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
+      <c r="D12">
+        <v>0.4</v>
+      </c>
+      <c r="E12">
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -621,13 +607,13 @@
         <v>100</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>0.4</v>
+      </c>
+      <c r="E13">
+        <v>0.08</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -640,11 +626,11 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
+      <c r="D14">
+        <v>0.4</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -657,11 +643,11 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+      <c r="E15">
+        <v>0.03</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -674,11 +660,11 @@
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -691,11 +677,11 @@
       <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
+      <c r="D17">
+        <v>0.3</v>
+      </c>
+      <c r="E17">
+        <v>0.02</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -706,13 +692,13 @@
         <v>100</v>
       </c>
       <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>0.3</v>
+      </c>
+      <c r="E18">
+        <v>0.02</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -723,13 +709,13 @@
         <v>100</v>
       </c>
       <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>0.35</v>
+      </c>
+      <c r="E19">
+        <v>0.02</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -740,13 +726,13 @@
         <v>100</v>
       </c>
       <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -759,11 +745,11 @@
       <c r="C21">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -776,11 +762,11 @@
       <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
+      <c r="D22">
+        <v>0.4</v>
+      </c>
+      <c r="E22">
+        <v>0.01</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -791,13 +777,13 @@
         <v>100</v>
       </c>
       <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
         <v>5</v>
+      </c>
+      <c r="D23">
+        <v>0.3</v>
+      </c>
+      <c r="E23">
+        <v>0.02</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -808,13 +794,13 @@
         <v>100</v>
       </c>
       <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>0.3</v>
+      </c>
+      <c r="E24">
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -825,13 +811,13 @@
         <v>100</v>
       </c>
       <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>0.4</v>
+      </c>
+      <c r="E25">
+        <v>0.05</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -842,13 +828,13 @@
         <v>100</v>
       </c>
       <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
         <v>5</v>
+      </c>
+      <c r="D26">
+        <v>0.5</v>
+      </c>
+      <c r="E26">
+        <v>0.08</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -861,11 +847,11 @@
       <c r="C27">
         <v>6</v>
       </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
+      <c r="D27">
+        <v>0.45</v>
+      </c>
+      <c r="E27">
+        <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -878,11 +864,11 @@
       <c r="C28">
         <v>6</v>
       </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
-        <v>7</v>
+      <c r="D28">
+        <v>0.4</v>
+      </c>
+      <c r="E28">
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -895,11 +881,11 @@
       <c r="C29">
         <v>6</v>
       </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
-        <v>7</v>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+      <c r="E29">
+        <v>0.02</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -912,37 +898,106 @@
       <c r="C30">
         <v>6</v>
       </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
+      <c r="D30">
+        <v>0.4</v>
+      </c>
+      <c r="E30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>0.4</v>
+      </c>
+      <c r="E31">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>0.8</v>
+      </c>
+      <c r="E32">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>0.65</v>
+      </c>
+      <c r="E33">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>100</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>0.6</v>
+      </c>
+      <c r="E34">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added Genie, tidied code, calculated new results
</commit_message>
<xml_diff>
--- a/code/params/100_graph_params.xlsx
+++ b/code/params/100_graph_params.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ku51015\CHMURA\mystuff\geaometricgraphproperties\code\params\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4D265-583C-4EA8-A2E0-FCA0992619CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="13570" windowWidth="13070" windowHeight="10910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10545" yWindow="13575" windowWidth="13065" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -42,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -82,7 +76,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -98,9 +92,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +132,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -172,7 +166,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -207,10 +200,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,16 +375,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -474,7 +466,7 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="E5">
         <v>0.08</v>
@@ -980,24 +972,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>